<commit_message>
add field Purpose for ProjectInfo
</commit_message>
<xml_diff>
--- a/SpecMaker/Resources/ExcelTemplates/Шаблон спецификации.xlsx
+++ b/SpecMaker/Resources/ExcelTemplates/Шаблон спецификации.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>Лист</t>
   </si>
@@ -118,6 +118,21 @@
   </si>
   <si>
     <t>СПЕЦИФИКАЦИЯ РУЧНОЙ АРМАТУРЫ</t>
+  </si>
+  <si>
+    <t>Иванов</t>
+  </si>
+  <si>
+    <t>Петров</t>
+  </si>
+  <si>
+    <t>Сидоров</t>
+  </si>
+  <si>
+    <t>Макаров</t>
+  </si>
+  <si>
+    <t>Трофимов</t>
   </si>
 </sst>
 </file>
@@ -1879,7 +1894,7 @@
   <dimension ref="B1:AA64"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" showWhiteSpace="0" view="pageBreakPreview" topLeftCell="I33" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="R48" sqref="R48:V50"/>
+      <selection activeCell="R51" sqref="R51:V54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -3252,14 +3267,16 @@
         <v>23</v>
       </c>
       <c r="K48" s="128"/>
-      <c r="L48" s="127"/>
+      <c r="L48" s="127" t="s">
+        <v>29</v>
+      </c>
       <c r="M48" s="129"/>
       <c r="N48" s="128"/>
       <c r="O48" s="33"/>
       <c r="P48" s="34"/>
       <c r="Q48" s="17" t="str">
         <f ca="1">CONCATENATE(IF(MONTH(TODAY())&lt;10,"0",""),MONTH(TODAY()),".",RIGHT(YEAR(TODAY()),2))</f>
-        <v>08.22</v>
+        <v>11.22</v>
       </c>
       <c r="R48" s="51"/>
       <c r="S48" s="52"/>
@@ -3292,14 +3309,16 @@
         <v>24</v>
       </c>
       <c r="K49" s="149"/>
-      <c r="L49" s="148"/>
+      <c r="L49" s="148" t="s">
+        <v>30</v>
+      </c>
       <c r="M49" s="156"/>
       <c r="N49" s="149"/>
       <c r="O49" s="31"/>
       <c r="P49" s="32"/>
       <c r="Q49" s="18" t="str">
         <f ca="1">Q48</f>
-        <v>08.22</v>
+        <v>11.22</v>
       </c>
       <c r="R49" s="54"/>
       <c r="S49" s="55"/>
@@ -3331,14 +3350,16 @@
         <v>27</v>
       </c>
       <c r="K50" s="149"/>
-      <c r="L50" s="148"/>
+      <c r="L50" s="148" t="s">
+        <v>31</v>
+      </c>
       <c r="M50" s="156"/>
       <c r="N50" s="149"/>
       <c r="O50" s="31"/>
       <c r="P50" s="32"/>
       <c r="Q50" s="18" t="str">
         <f ca="1">Q48</f>
-        <v>08.22</v>
+        <v>11.22</v>
       </c>
       <c r="R50" s="57"/>
       <c r="S50" s="58"/>
@@ -3392,14 +3413,16 @@
         <v>25</v>
       </c>
       <c r="K52" s="153"/>
-      <c r="L52" s="152"/>
+      <c r="L52" s="152" t="s">
+        <v>32</v>
+      </c>
       <c r="M52" s="158"/>
       <c r="N52" s="153"/>
       <c r="O52" s="119"/>
       <c r="P52" s="35"/>
       <c r="Q52" s="60" t="str">
         <f ca="1">Q48</f>
-        <v>08.22</v>
+        <v>11.22</v>
       </c>
       <c r="R52" s="62"/>
       <c r="S52" s="63"/>
@@ -3451,14 +3474,16 @@
         <v>26</v>
       </c>
       <c r="K54" s="151"/>
-      <c r="L54" s="150"/>
+      <c r="L54" s="150" t="s">
+        <v>33</v>
+      </c>
       <c r="M54" s="157"/>
       <c r="N54" s="151"/>
       <c r="O54" s="37"/>
       <c r="P54" s="38"/>
       <c r="Q54" s="30" t="str">
         <f ca="1">Q48</f>
-        <v>08.22</v>
+        <v>11.22</v>
       </c>
       <c r="R54" s="65"/>
       <c r="S54" s="66"/>

</xml_diff>